<commit_message>
Add item counts and deliveries [HW3]
</commit_message>
<xml_diff>
--- a/Stats/Stats (Vincent & Joseph Scavetta).xlsx
+++ b/Stats/Stats (Vincent & Joseph Scavetta).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\OneDrive\School\Masters\Rowan Year 1 (2018-2019)\Spring 2019\Data Warehousing\DataWarehousingHW1\Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{7B227FF9-2816-44A7-9977-4BB74AC64DA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{17458C29-9AD3-4AEA-B5EC-581DF31ED841}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{7B227FF9-2816-44A7-9977-4BB74AC64DA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{EEAE14A5-9EE5-48B7-A2BC-CD4C68CBAF75}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32910" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>Milk</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Daily Actuals</t>
+  </si>
+  <si>
+    <t>Daily Per Item</t>
   </si>
 </sst>
 </file>
@@ -243,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -292,6 +295,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,8 +622,8 @@
         <v>1200</v>
       </c>
       <c r="C2" s="4">
-        <f>AVERAGE(B2,1250)*(5/7)+D2*(2/7)</f>
-        <v>1246.4285714285713</v>
+        <f>AVERAGE(B2,1250)*(5/7)+AVERAGE(1250,D2)*(2/7)</f>
+        <v>1239.2857142857142</v>
       </c>
       <c r="D2" s="5">
         <v>1300</v>
@@ -651,7 +660,7 @@
       </c>
       <c r="C4" s="4">
         <f>C2*0.7</f>
-        <v>872.49999999999989</v>
+        <v>867.49999999999989</v>
       </c>
       <c r="D4" s="5">
         <f>D2*0.7</f>
@@ -674,7 +683,7 @@
       </c>
       <c r="C5" s="8">
         <f>C4*0.5+(C2*0.3*0.05)</f>
-        <v>454.9464285714285</v>
+        <v>452.33928571428567</v>
       </c>
       <c r="D5" s="9">
         <f>D4*0.5+(D2*0.3*0.05)</f>
@@ -697,7 +706,7 @@
       </c>
       <c r="C6" s="8">
         <f>C2*0.2</f>
-        <v>249.28571428571428</v>
+        <v>247.85714285714286</v>
       </c>
       <c r="D6" s="9">
         <f>D2*0.2</f>
@@ -720,7 +729,7 @@
       </c>
       <c r="C7" s="8">
         <f>C6*0.8+(C2*0.8*0.01)</f>
-        <v>209.4</v>
+        <v>208.20000000000002</v>
       </c>
       <c r="D7" s="9">
         <f>D6*0.8+(D2*0.8*0.01)</f>
@@ -743,7 +752,7 @@
       </c>
       <c r="C8" s="8">
         <f>C2*0.5</f>
-        <v>623.21428571428567</v>
+        <v>619.64285714285711</v>
       </c>
       <c r="D8" s="9">
         <f>D2*0.5</f>
@@ -766,7 +775,7 @@
       </c>
       <c r="C9" s="8">
         <f>C2*0.1</f>
-        <v>124.64285714285714</v>
+        <v>123.92857142857143</v>
       </c>
       <c r="D9" s="9">
         <f>D2*0.1</f>
@@ -789,7 +798,7 @@
       </c>
       <c r="C10" s="8">
         <f>C9*0.9+(C2*0.9*0.05)</f>
-        <v>168.26785714285714</v>
+        <v>167.30357142857144</v>
       </c>
       <c r="D10" s="9">
         <f>D9*0.9+(D2*0.9*0.05)</f>
@@ -807,15 +816,14 @@
         <v>6</v>
       </c>
       <c r="B11" s="10">
-        <f>B3*B2</f>
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="C11" s="10">
-        <f>C3*C2</f>
-        <v>41132.142857142855</v>
+        <f>(C3*C2)-SUM(C4:C10)</f>
+        <v>38209.657142857141</v>
       </c>
       <c r="D11" s="11">
-        <f>D3*D2</f>
+        <f>(D3*D2)</f>
         <v>84500</v>
       </c>
       <c r="F11" s="16" t="s">
@@ -826,14 +834,85 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="17">
+        <f>C4/6</f>
+        <v>144.58333333333331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="17">
+        <f>C5/93</f>
+        <v>4.8638632872503837</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="17">
+        <f>C6/162</f>
+        <v>1.5299823633156966</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="17">
+        <f>C7/82</f>
+        <v>2.5390243902439025</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="17">
+        <f>C8/48</f>
+        <v>12.90922619047619</v>
+      </c>
       <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="17">
+        <f>C9/20</f>
+        <v>6.1964285714285712</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="17">
+        <f>C10/4</f>
+        <v>41.825892857142861</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="18">
+        <f>C11/(2075-415)</f>
+        <v>23.01786574870912</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>